<commit_message>
[29.03] 2115 Creates all views, setting logic. Stopping on async commands
</commit_message>
<xml_diff>
--- a/Console/Main2.xlsx
+++ b/Console/Main2.xlsx
@@ -1880,9 +1880,9 @@
   <dimension ref="A1:K254"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -2065,21 +2065,6 @@
       <c r="F8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="3">
-        <v>47</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>1</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3">
-        <v>13</v>
-      </c>
     </row>
     <row r="9" outlineLevel="2">
       <c r="A9" s="16">
@@ -2124,13 +2109,13 @@
         <v>0</v>
       </c>
       <c r="H10" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I10" s="3">
         <v>0</v>
       </c>
       <c r="J10" s="3">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="K10" s="3">
         <v>0</v>
@@ -2155,6 +2140,21 @@
       <c r="F11" s="14" t="s">
         <v>40</v>
       </c>
+      <c r="G11" s="3">
+        <v>80</v>
+      </c>
+      <c r="H11" s="3">
+        <v>16.5</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1753</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" outlineLevel="2">
       <c r="A12" s="16">
@@ -2175,21 +2175,6 @@
       <c r="F12" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="3">
-        <v>282</v>
-      </c>
-      <c r="H12" s="3">
-        <v>4.3000000000000007</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0</v>
-      </c>
-      <c r="J12" s="3">
-        <v>169</v>
-      </c>
-      <c r="K12" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" outlineLevel="2">
       <c r="A13" s="16">
@@ -2211,13 +2196,13 @@
         <v>45</v>
       </c>
       <c r="G13" s="3">
-        <v>431</v>
+        <v>5</v>
       </c>
       <c r="H13" s="3">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="I13" s="3">
-        <v>359</v>
+        <v>29</v>
       </c>
       <c r="J13" s="3">
         <v>0</v>
@@ -2249,13 +2234,13 @@
         <v>0</v>
       </c>
       <c r="H14" s="3">
-        <v>72.5</v>
+        <v>43</v>
       </c>
       <c r="I14" s="3">
         <v>0</v>
       </c>
       <c r="J14" s="3">
-        <v>419</v>
+        <v>246</v>
       </c>
       <c r="K14" s="3">
         <v>0</v>
@@ -2284,13 +2269,13 @@
         <v>0</v>
       </c>
       <c r="H15" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I15" s="3">
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="K15" s="3">
         <v>0</v>
@@ -2315,21 +2300,6 @@
       <c r="F16" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>20</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0</v>
-      </c>
-      <c r="J16" s="3">
-        <v>40</v>
-      </c>
-      <c r="K16" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" outlineLevel="2">
       <c r="A17" s="16">
@@ -2371,13 +2341,13 @@
         <v>57</v>
       </c>
       <c r="G18" s="3">
-        <v>1473</v>
+        <v>1135</v>
       </c>
       <c r="H18" s="3">
         <v>0</v>
       </c>
       <c r="I18" s="3">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="J18" s="3">
         <v>0</v>
@@ -2406,13 +2376,13 @@
         <v>60</v>
       </c>
       <c r="G19" s="3">
-        <v>666</v>
+        <v>608</v>
       </c>
       <c r="H19" s="3">
         <v>0</v>
       </c>
       <c r="I19" s="3">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J19" s="3">
         <v>0</v>
@@ -2441,16 +2411,16 @@
         <v>62</v>
       </c>
       <c r="G20" s="3">
-        <v>538</v>
+        <v>103</v>
       </c>
       <c r="H20" s="3">
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="I20" s="3">
         <v>0</v>
       </c>
       <c r="J20" s="3">
-        <v>155</v>
+        <v>36</v>
       </c>
       <c r="K20" s="3">
         <v>0</v>
@@ -2476,16 +2446,16 @@
         <v>63</v>
       </c>
       <c r="G21" s="3">
-        <v>243</v>
+        <v>763</v>
       </c>
       <c r="H21" s="3">
-        <v>1</v>
+        <v>6.5</v>
       </c>
       <c r="I21" s="3">
         <v>0</v>
       </c>
       <c r="J21" s="3">
-        <v>62</v>
+        <v>210</v>
       </c>
       <c r="K21" s="3">
         <v>0</v>
@@ -2511,7 +2481,7 @@
         <v>66</v>
       </c>
       <c r="G22" s="3">
-        <v>269</v>
+        <v>341</v>
       </c>
       <c r="H22" s="3">
         <v>0</v>
@@ -2520,7 +2490,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="K22" s="3">
         <v>0</v>
@@ -2546,13 +2516,13 @@
         <v>68</v>
       </c>
       <c r="G23" s="3">
-        <v>592</v>
+        <v>771</v>
       </c>
       <c r="H23" s="3">
         <v>0</v>
       </c>
       <c r="I23" s="3">
-        <v>68</v>
+        <v>84.660000000000011</v>
       </c>
       <c r="J23" s="3">
         <v>0</v>
@@ -2581,13 +2551,13 @@
         <v>69</v>
       </c>
       <c r="G24" s="3">
-        <v>1454</v>
+        <v>1416</v>
       </c>
       <c r="H24" s="3">
         <v>0</v>
       </c>
       <c r="I24" s="3">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J24" s="3">
         <v>0</v>
@@ -2616,13 +2586,13 @@
         <v>71</v>
       </c>
       <c r="G25" s="3">
-        <v>2305</v>
+        <v>2677</v>
       </c>
       <c r="H25" s="3">
         <v>0</v>
       </c>
       <c r="I25" s="3">
-        <v>412</v>
+        <v>467</v>
       </c>
       <c r="J25" s="3">
         <v>0</v>
@@ -2651,13 +2621,13 @@
         <v>73</v>
       </c>
       <c r="G26" s="3">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
       </c>
       <c r="I26" s="3">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J26" s="3">
         <v>0</v>
@@ -2686,13 +2656,13 @@
         <v>75</v>
       </c>
       <c r="G27" s="3">
-        <v>503</v>
+        <v>550</v>
       </c>
       <c r="H27" s="3">
         <v>0</v>
       </c>
       <c r="I27" s="3">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="J27" s="3">
         <v>0</v>
@@ -2720,21 +2690,6 @@
       <c r="F28" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G28" s="3">
-        <v>51</v>
-      </c>
-      <c r="H28" s="3">
-        <v>0</v>
-      </c>
-      <c r="I28" s="3">
-        <v>5</v>
-      </c>
-      <c r="J28" s="3">
-        <v>0</v>
-      </c>
-      <c r="K28" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="29" ht="12.75" customHeight="1" outlineLevel="2">
       <c r="A29" s="16">
@@ -2756,13 +2711,13 @@
         <v>78</v>
       </c>
       <c r="G29" s="3">
-        <v>707</v>
+        <v>582</v>
       </c>
       <c r="H29" s="3">
         <v>0</v>
       </c>
       <c r="I29" s="3">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J29" s="3">
         <v>0</v>
@@ -2791,13 +2746,13 @@
         <v>79</v>
       </c>
       <c r="G30" s="3">
+        <v>1324</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
         <v>123</v>
-      </c>
-      <c r="H30" s="3">
-        <v>0</v>
-      </c>
-      <c r="I30" s="3">
-        <v>12</v>
       </c>
       <c r="J30" s="3">
         <v>0</v>
@@ -2826,13 +2781,13 @@
         <v>80</v>
       </c>
       <c r="G31" s="3">
-        <v>661</v>
+        <v>524</v>
       </c>
       <c r="H31" s="3">
         <v>0</v>
       </c>
       <c r="I31" s="3">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="J31" s="3">
         <v>0</v>
@@ -2860,21 +2815,6 @@
       <c r="F32" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="G32" s="3">
-        <v>836</v>
-      </c>
-      <c r="H32" s="3">
-        <v>0</v>
-      </c>
-      <c r="I32" s="3">
-        <v>94</v>
-      </c>
-      <c r="J32" s="3">
-        <v>0</v>
-      </c>
-      <c r="K32" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="33" ht="12.75" customHeight="1" outlineLevel="2">
       <c r="A33" s="16">
@@ -2896,13 +2836,13 @@
         <v>83</v>
       </c>
       <c r="G33" s="3">
-        <v>899</v>
+        <v>1056</v>
       </c>
       <c r="H33" s="3">
         <v>0</v>
       </c>
       <c r="I33" s="3">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="J33" s="3">
         <v>0</v>
@@ -2931,13 +2871,13 @@
         <v>85</v>
       </c>
       <c r="G34" s="3">
-        <v>462</v>
+        <v>1116</v>
       </c>
       <c r="H34" s="3">
         <v>0</v>
       </c>
       <c r="I34" s="3">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="J34" s="3">
         <v>0</v>
@@ -2966,16 +2906,16 @@
         <v>87</v>
       </c>
       <c r="G35" s="3">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="H35" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I35" s="3">
         <v>0</v>
       </c>
       <c r="J35" s="3">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="K35" s="3">
         <v>0</v>
@@ -3001,16 +2941,16 @@
         <v>89</v>
       </c>
       <c r="G36" s="3">
-        <v>676</v>
+        <v>762</v>
       </c>
       <c r="H36" s="3">
-        <v>24.5</v>
+        <v>23.5</v>
       </c>
       <c r="I36" s="3">
         <v>0</v>
       </c>
       <c r="J36" s="3">
-        <v>402</v>
+        <v>416</v>
       </c>
       <c r="K36" s="3">
         <v>0</v>
@@ -3035,6 +2975,21 @@
       <c r="F37" s="14" t="s">
         <v>91</v>
       </c>
+      <c r="G37" s="3">
+        <v>591</v>
+      </c>
+      <c r="H37" s="3">
+        <v>17</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0</v>
+      </c>
+      <c r="J37" s="3">
+        <v>322</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" ht="12.75" customHeight="1" outlineLevel="2">
       <c r="A38" s="16">
@@ -3055,21 +3010,6 @@
       <c r="F38" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G38" s="3">
-        <v>16</v>
-      </c>
-      <c r="H38" s="3">
-        <v>0</v>
-      </c>
-      <c r="I38" s="3">
-        <v>0</v>
-      </c>
-      <c r="J38" s="3">
-        <v>6</v>
-      </c>
-      <c r="K38" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="39" ht="12.75" customHeight="1" outlineLevel="2">
       <c r="A39" s="16">
@@ -3091,13 +3031,13 @@
         <v>95</v>
       </c>
       <c r="G39" s="3">
-        <v>776</v>
+        <v>322</v>
       </c>
       <c r="H39" s="3">
         <v>0</v>
       </c>
       <c r="I39" s="3">
-        <v>158</v>
+        <v>65</v>
       </c>
       <c r="J39" s="3">
         <v>0</v>
@@ -3126,13 +3066,13 @@
         <v>97</v>
       </c>
       <c r="G40" s="3">
-        <v>290</v>
+        <v>482</v>
       </c>
       <c r="H40" s="3">
         <v>0</v>
       </c>
       <c r="I40" s="3">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="J40" s="3">
         <v>0</v>
@@ -3161,13 +3101,13 @@
         <v>100</v>
       </c>
       <c r="G41" s="3">
-        <v>287</v>
+        <v>745</v>
       </c>
       <c r="H41" s="3">
         <v>0</v>
       </c>
       <c r="I41" s="3">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="J41" s="3">
         <v>0</v>
@@ -3196,13 +3136,13 @@
         <v>103</v>
       </c>
       <c r="G42" s="3">
-        <v>141</v>
+        <v>461</v>
       </c>
       <c r="H42" s="3">
         <v>0</v>
       </c>
       <c r="I42" s="3">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="J42" s="3">
         <v>0</v>
@@ -3231,13 +3171,13 @@
         <v>104</v>
       </c>
       <c r="G43" s="3">
-        <v>1248</v>
+        <v>162</v>
       </c>
       <c r="H43" s="3">
         <v>0</v>
       </c>
       <c r="I43" s="3">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="J43" s="3">
         <v>0</v>
@@ -3265,6 +3205,21 @@
       <c r="F44" s="14" t="s">
         <v>107</v>
       </c>
+      <c r="G44" s="3">
+        <v>333</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0</v>
+      </c>
+      <c r="J44" s="3">
+        <v>116</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" ht="12.75" customHeight="1" outlineLevel="2">
       <c r="A45" s="16">
@@ -3286,19 +3241,19 @@
         <v>109</v>
       </c>
       <c r="G45" s="3">
-        <v>952</v>
+        <v>1060</v>
       </c>
       <c r="H45" s="3">
         <v>0</v>
       </c>
       <c r="I45" s="3">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J45" s="3">
         <v>0</v>
       </c>
       <c r="K45" s="3">
-        <v>153</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" ht="12.75" customHeight="1" outlineLevel="2">
@@ -3321,13 +3276,13 @@
         <v>112</v>
       </c>
       <c r="G46" s="3">
-        <v>382</v>
+        <v>103</v>
       </c>
       <c r="H46" s="3">
         <v>0</v>
       </c>
       <c r="I46" s="3">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="J46" s="3">
         <v>0</v>
@@ -3356,13 +3311,13 @@
         <v>113</v>
       </c>
       <c r="G47" s="3">
-        <v>329</v>
+        <v>2076</v>
       </c>
       <c r="H47" s="3">
         <v>0</v>
       </c>
       <c r="I47" s="3">
-        <v>35.25</v>
+        <v>228</v>
       </c>
       <c r="J47" s="3">
         <v>0</v>
@@ -3391,13 +3346,13 @@
         <v>114</v>
       </c>
       <c r="G48" s="3">
-        <v>1352</v>
+        <v>821</v>
       </c>
       <c r="H48" s="3">
         <v>0</v>
       </c>
       <c r="I48" s="3">
-        <v>135</v>
+        <v>78</v>
       </c>
       <c r="J48" s="3">
         <v>0</v>
@@ -3426,13 +3381,13 @@
         <v>115</v>
       </c>
       <c r="G49" s="3">
-        <v>1642</v>
+        <v>1847</v>
       </c>
       <c r="H49" s="3">
         <v>0</v>
       </c>
       <c r="I49" s="3">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="J49" s="3">
         <v>0</v>
@@ -3461,13 +3416,13 @@
         <v>116</v>
       </c>
       <c r="G50" s="3">
-        <v>798</v>
+        <v>1002</v>
       </c>
       <c r="H50" s="3">
         <v>0</v>
       </c>
       <c r="I50" s="3">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="J50" s="3">
         <v>0</v>
@@ -3496,13 +3451,13 @@
         <v>117</v>
       </c>
       <c r="G51" s="3">
-        <v>781</v>
+        <v>823</v>
       </c>
       <c r="H51" s="3">
         <v>0</v>
       </c>
       <c r="I51" s="3">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J51" s="3">
         <v>0</v>
@@ -3530,21 +3485,6 @@
       <c r="F52" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="G52" s="3">
-        <v>109</v>
-      </c>
-      <c r="H52" s="3">
-        <v>0</v>
-      </c>
-      <c r="I52" s="3">
-        <v>10</v>
-      </c>
-      <c r="J52" s="3">
-        <v>0</v>
-      </c>
-      <c r="K52" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="53" ht="12.75" customHeight="1" outlineLevel="2">
       <c r="A53" s="16">
@@ -3585,21 +3525,6 @@
       <c r="F54" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="G54" s="3">
-        <v>80</v>
-      </c>
-      <c r="H54" s="3">
-        <v>0</v>
-      </c>
-      <c r="I54" s="3">
-        <v>3</v>
-      </c>
-      <c r="J54" s="3">
-        <v>0</v>
-      </c>
-      <c r="K54" s="3">
-        <v>27</v>
-      </c>
     </row>
     <row r="55" ht="12.75" customHeight="1" outlineLevel="2">
       <c r="A55" s="16">
@@ -3621,7 +3546,7 @@
         <v>124</v>
       </c>
       <c r="G55" s="3">
-        <v>1262</v>
+        <v>1855</v>
       </c>
       <c r="H55" s="3">
         <v>0</v>
@@ -3630,7 +3555,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="3">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="K55" s="3">
         <v>0</v>
@@ -3655,6 +3580,21 @@
       <c r="F56" s="11" t="s">
         <v>126</v>
       </c>
+      <c r="G56" s="3">
+        <v>1150</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0</v>
+      </c>
+      <c r="J56" s="3">
+        <v>396</v>
+      </c>
+      <c r="K56" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" ht="12.75" customHeight="1" outlineLevel="2">
       <c r="A57" s="16">
@@ -3696,7 +3636,7 @@
         <v>132</v>
       </c>
       <c r="G58" s="3">
-        <v>1627</v>
+        <v>1184</v>
       </c>
       <c r="H58" s="3">
         <v>0</v>
@@ -3705,7 +3645,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="3">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="K58" s="3">
         <v>0</v>
@@ -3731,13 +3671,13 @@
         <v>136</v>
       </c>
       <c r="G59" s="3">
-        <v>346</v>
+        <v>1270</v>
       </c>
       <c r="H59" s="3">
         <v>0</v>
       </c>
       <c r="I59" s="3">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="J59" s="3">
         <v>0</v>
@@ -3766,13 +3706,13 @@
         <v>139</v>
       </c>
       <c r="G60" s="3">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="H60" s="3">
         <v>0</v>
       </c>
       <c r="I60" s="3">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="J60" s="3">
         <v>0</v>
@@ -3795,19 +3735,19 @@
       <c r="E61" s="20"/>
       <c r="F61" s="8"/>
       <c r="G61" s="7">
-        <v>26179</v>
+        <v>30736</v>
       </c>
       <c r="H61" s="7">
-        <v>183.8</v>
+        <v>165.5</v>
       </c>
       <c r="I61" s="7">
-        <v>2754.25</v>
+        <v>2757.66</v>
       </c>
       <c r="J61" s="7">
-        <v>1902</v>
+        <v>4316</v>
       </c>
       <c r="K61" s="7">
-        <v>193</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" outlineLevel="2">
@@ -3830,7 +3770,7 @@
         <v>143</v>
       </c>
       <c r="G62" s="3">
-        <v>703</v>
+        <v>797</v>
       </c>
       <c r="H62" s="3">
         <v>0</v>
@@ -3839,7 +3779,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="3">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="K62" s="3">
         <v>0</v>
@@ -3865,13 +3805,13 @@
         <v>145</v>
       </c>
       <c r="G63" s="3">
-        <v>293</v>
+        <v>548</v>
       </c>
       <c r="H63" s="3">
         <v>0</v>
       </c>
       <c r="I63" s="3">
-        <v>28.430000000000007</v>
+        <v>51.580000000000005</v>
       </c>
       <c r="J63" s="3">
         <v>0</v>
@@ -3940,13 +3880,13 @@
         <v>152</v>
       </c>
       <c r="G66" s="3">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
       </c>
       <c r="I66" s="3">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="J66" s="3">
         <v>0</v>
@@ -3974,6 +3914,21 @@
       <c r="F67" s="17" t="s">
         <v>154</v>
       </c>
+      <c r="G67" s="3">
+        <v>210</v>
+      </c>
+      <c r="H67" s="3">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3">
+        <v>39</v>
+      </c>
+      <c r="J67" s="3">
+        <v>0</v>
+      </c>
+      <c r="K67" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" outlineLevel="2">
       <c r="A68" s="16">
@@ -3995,13 +3950,13 @@
         <v>156</v>
       </c>
       <c r="G68" s="3">
-        <v>129</v>
+        <v>571</v>
       </c>
       <c r="H68" s="3">
         <v>0</v>
       </c>
       <c r="I68" s="3">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="J68" s="3">
         <v>0</v>
@@ -4030,13 +3985,13 @@
         <v>158</v>
       </c>
       <c r="G69" s="3">
-        <v>123</v>
+        <v>547</v>
       </c>
       <c r="H69" s="3">
         <v>0</v>
       </c>
       <c r="I69" s="3">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="J69" s="3">
         <v>0</v>
@@ -4065,7 +4020,7 @@
         <v>161</v>
       </c>
       <c r="G70" s="3">
-        <v>556</v>
+        <v>1409</v>
       </c>
       <c r="H70" s="3">
         <v>0</v>
@@ -4074,7 +4029,7 @@
         <v>0</v>
       </c>
       <c r="J70" s="3">
-        <v>124.88</v>
+        <v>307.58</v>
       </c>
       <c r="K70" s="3">
         <v>0</v>
@@ -4100,7 +4055,7 @@
         <v>162</v>
       </c>
       <c r="G71" s="3">
-        <v>244</v>
+        <v>1113</v>
       </c>
       <c r="H71" s="3">
         <v>0</v>
@@ -4109,7 +4064,7 @@
         <v>0</v>
       </c>
       <c r="J71" s="3">
-        <v>54.79</v>
+        <v>241.40000000000003</v>
       </c>
       <c r="K71" s="3">
         <v>0</v>
@@ -4135,7 +4090,7 @@
         <v>163</v>
       </c>
       <c r="G72" s="3">
-        <v>249</v>
+        <v>573</v>
       </c>
       <c r="H72" s="3">
         <v>0</v>
@@ -4144,7 +4099,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="3">
-        <v>55.92</v>
+        <v>125.32</v>
       </c>
       <c r="K72" s="3">
         <v>0</v>
@@ -4169,6 +4124,21 @@
       <c r="F73" s="11" t="s">
         <v>166</v>
       </c>
+      <c r="G73" s="3">
+        <v>338</v>
+      </c>
+      <c r="H73" s="3">
+        <v>0</v>
+      </c>
+      <c r="I73" s="3">
+        <v>0</v>
+      </c>
+      <c r="J73" s="3">
+        <v>53.12</v>
+      </c>
+      <c r="K73" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" outlineLevel="2">
       <c r="A74" s="16">
@@ -4190,7 +4160,7 @@
         <v>167</v>
       </c>
       <c r="G74" s="3">
-        <v>316</v>
+        <v>875</v>
       </c>
       <c r="H74" s="3">
         <v>0</v>
@@ -4199,7 +4169,7 @@
         <v>0</v>
       </c>
       <c r="J74" s="3">
-        <v>70.97999999999999</v>
+        <v>190.31</v>
       </c>
       <c r="K74" s="3">
         <v>0</v>
@@ -4225,16 +4195,16 @@
         <v>169</v>
       </c>
       <c r="G75" s="3">
-        <v>437</v>
+        <v>346</v>
       </c>
       <c r="H75" s="3">
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="I75" s="3">
         <v>0</v>
       </c>
       <c r="J75" s="3">
-        <v>261.13</v>
+        <v>211.40000000000003</v>
       </c>
       <c r="K75" s="3">
         <v>0</v>
@@ -4260,7 +4230,7 @@
         <v>171</v>
       </c>
       <c r="G76" s="3">
-        <v>391</v>
+        <v>732</v>
       </c>
       <c r="H76" s="3">
         <v>0</v>
@@ -4269,7 +4239,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="3">
-        <v>87.83</v>
+        <v>160.76000000000002</v>
       </c>
       <c r="K76" s="3">
         <v>0</v>
@@ -4295,13 +4265,13 @@
         <v>173</v>
       </c>
       <c r="G77" s="3">
-        <v>323</v>
+        <v>525</v>
       </c>
       <c r="H77" s="3">
         <v>0</v>
       </c>
       <c r="I77" s="3">
-        <v>63.690000000000005</v>
+        <v>101.29</v>
       </c>
       <c r="J77" s="3">
         <v>0</v>
@@ -4330,7 +4300,7 @@
         <v>175</v>
       </c>
       <c r="G78" s="3">
-        <v>481</v>
+        <v>724</v>
       </c>
       <c r="H78" s="3">
         <v>0</v>
@@ -4339,7 +4309,7 @@
         <v>0</v>
       </c>
       <c r="J78" s="3">
-        <v>96.840000000000018</v>
+        <v>139.89999999999998</v>
       </c>
       <c r="K78" s="3">
         <v>0</v>
@@ -4365,7 +4335,7 @@
         <v>178</v>
       </c>
       <c r="G79" s="3">
-        <v>258</v>
+        <v>1330</v>
       </c>
       <c r="H79" s="3">
         <v>0</v>
@@ -4374,7 +4344,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="3">
-        <v>42.490000000000009</v>
+        <v>220.27</v>
       </c>
       <c r="K79" s="3">
         <v>0</v>
@@ -4400,7 +4370,7 @@
         <v>181</v>
       </c>
       <c r="G80" s="3">
-        <v>540</v>
+        <v>1531</v>
       </c>
       <c r="H80" s="3">
         <v>0</v>
@@ -4409,7 +4379,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="3">
-        <v>74</v>
+        <v>206</v>
       </c>
       <c r="K80" s="3">
         <v>0</v>
@@ -4434,6 +4404,21 @@
       <c r="F81" s="19" t="s">
         <v>184</v>
       </c>
+      <c r="G81" s="3">
+        <v>247</v>
+      </c>
+      <c r="H81" s="3">
+        <v>0</v>
+      </c>
+      <c r="I81" s="3">
+        <v>0</v>
+      </c>
+      <c r="J81" s="3">
+        <v>57</v>
+      </c>
+      <c r="K81" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" outlineLevel="2">
       <c r="A82" s="16">
@@ -4455,19 +4440,19 @@
         <v>185</v>
       </c>
       <c r="G82" s="3">
-        <v>1408</v>
+        <v>1188</v>
       </c>
       <c r="H82" s="3">
         <v>0</v>
       </c>
       <c r="I82" s="3">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J82" s="3">
         <v>0</v>
       </c>
       <c r="K82" s="3">
-        <v>338</v>
+        <v>276</v>
       </c>
     </row>
     <row r="83" outlineLevel="2">
@@ -4490,13 +4475,13 @@
         <v>188</v>
       </c>
       <c r="G83" s="3">
-        <v>1391</v>
+        <v>1477</v>
       </c>
       <c r="H83" s="3">
         <v>0</v>
       </c>
       <c r="I83" s="3">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="J83" s="3">
         <v>0</v>
@@ -4524,6 +4509,21 @@
       <c r="F84" s="17" t="s">
         <v>189</v>
       </c>
+      <c r="G84" s="3">
+        <v>251</v>
+      </c>
+      <c r="H84" s="3">
+        <v>0</v>
+      </c>
+      <c r="I84" s="3">
+        <v>0</v>
+      </c>
+      <c r="J84" s="3">
+        <v>60</v>
+      </c>
+      <c r="K84" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" outlineLevel="2">
       <c r="A85" s="16">
@@ -4544,6 +4544,21 @@
       <c r="F85" s="19" t="s">
         <v>190</v>
       </c>
+      <c r="G85" s="3">
+        <v>1957</v>
+      </c>
+      <c r="H85" s="3">
+        <v>0</v>
+      </c>
+      <c r="I85" s="3">
+        <v>0</v>
+      </c>
+      <c r="J85" s="3">
+        <v>437</v>
+      </c>
+      <c r="K85" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="86" outlineLevel="2">
       <c r="A86" s="16">
@@ -4564,6 +4579,21 @@
       <c r="F86" s="19" t="s">
         <v>192</v>
       </c>
+      <c r="G86" s="3">
+        <v>1770</v>
+      </c>
+      <c r="H86" s="3">
+        <v>0</v>
+      </c>
+      <c r="I86" s="3">
+        <v>15</v>
+      </c>
+      <c r="J86" s="3">
+        <v>0</v>
+      </c>
+      <c r="K86" s="3">
+        <v>363</v>
+      </c>
     </row>
     <row r="87" outlineLevel="2">
       <c r="A87" s="16">
@@ -4584,6 +4614,21 @@
       <c r="F87" s="19" t="s">
         <v>194</v>
       </c>
+      <c r="G87" s="3">
+        <v>1367</v>
+      </c>
+      <c r="H87" s="3">
+        <v>0</v>
+      </c>
+      <c r="I87" s="3">
+        <v>0</v>
+      </c>
+      <c r="J87" s="3">
+        <v>127</v>
+      </c>
+      <c r="K87" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="88" outlineLevel="2">
       <c r="A88" s="16">
@@ -4605,19 +4650,19 @@
         <v>197</v>
       </c>
       <c r="G88" s="3">
-        <v>558</v>
+        <v>1110</v>
       </c>
       <c r="H88" s="3">
         <v>0</v>
       </c>
       <c r="I88" s="3">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="J88" s="3">
         <v>0</v>
       </c>
       <c r="K88" s="3">
-        <v>111</v>
+        <v>213</v>
       </c>
     </row>
     <row r="89" outlineLevel="2">
@@ -4640,7 +4685,7 @@
         <v>198</v>
       </c>
       <c r="G89" s="3">
-        <v>1132</v>
+        <v>1079</v>
       </c>
       <c r="H89" s="3">
         <v>0</v>
@@ -4649,7 +4694,7 @@
         <v>0</v>
       </c>
       <c r="J89" s="3">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="K89" s="3">
         <v>0</v>
@@ -4675,7 +4720,7 @@
         <v>199</v>
       </c>
       <c r="G90" s="3">
-        <v>658</v>
+        <v>1046</v>
       </c>
       <c r="H90" s="3">
         <v>0</v>
@@ -4684,7 +4729,7 @@
         <v>0</v>
       </c>
       <c r="J90" s="3">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="K90" s="3">
         <v>0</v>
@@ -4709,6 +4754,21 @@
       <c r="F91" s="19" t="s">
         <v>201</v>
       </c>
+      <c r="G91" s="3">
+        <v>1077</v>
+      </c>
+      <c r="H91" s="3">
+        <v>0</v>
+      </c>
+      <c r="I91" s="3">
+        <v>15</v>
+      </c>
+      <c r="J91" s="3">
+        <v>0</v>
+      </c>
+      <c r="K91" s="3">
+        <v>252</v>
+      </c>
     </row>
     <row r="92" outlineLevel="2">
       <c r="A92" s="16">
@@ -4730,7 +4790,7 @@
         <v>204</v>
       </c>
       <c r="G92" s="3">
-        <v>1180</v>
+        <v>1155</v>
       </c>
       <c r="H92" s="3">
         <v>0</v>
@@ -4739,7 +4799,7 @@
         <v>0</v>
       </c>
       <c r="J92" s="3">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="K92" s="3">
         <v>0</v>
@@ -4759,19 +4819,19 @@
       <c r="E93" s="20"/>
       <c r="F93" s="8"/>
       <c r="G93" s="7">
-        <v>11492</v>
+        <v>26072</v>
       </c>
       <c r="H93" s="7">
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="I93" s="7">
-        <v>341.12</v>
+        <v>652.87000000000012</v>
       </c>
       <c r="J93" s="7">
-        <v>1207.8600000000001</v>
+        <v>2901.06</v>
       </c>
       <c r="K93" s="7">
-        <v>449</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="94" hidden="1" outlineLevel="2">
@@ -4794,13 +4854,13 @@
         <v>207</v>
       </c>
       <c r="G94" s="3">
-        <v>1376</v>
+        <v>1020</v>
       </c>
       <c r="H94" s="3">
         <v>0</v>
       </c>
       <c r="I94" s="3">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="J94" s="3">
         <v>0</v>
@@ -4823,13 +4883,13 @@
       <c r="E95" s="20"/>
       <c r="F95" s="8"/>
       <c r="G95" s="7">
-        <v>1376</v>
+        <v>1020</v>
       </c>
       <c r="H95" s="7">
         <v>0</v>
       </c>
       <c r="I95" s="7">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="J95" s="7">
         <v>0</v>
@@ -4858,13 +4918,13 @@
         <v>210</v>
       </c>
       <c r="G96" s="3">
-        <v>843</v>
+        <v>1011</v>
       </c>
       <c r="H96" s="3">
         <v>0</v>
       </c>
       <c r="I96" s="3">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="J96" s="3">
         <v>0</v>
@@ -4893,13 +4953,13 @@
         <v>212</v>
       </c>
       <c r="G97" s="3">
-        <v>816</v>
+        <v>674</v>
       </c>
       <c r="H97" s="3">
         <v>0</v>
       </c>
       <c r="I97" s="3">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="J97" s="3">
         <v>0</v>
@@ -4922,13 +4982,13 @@
       <c r="E98" s="20"/>
       <c r="F98" s="8"/>
       <c r="G98" s="7">
-        <v>1659</v>
+        <v>1685</v>
       </c>
       <c r="H98" s="7">
         <v>0</v>
       </c>
       <c r="I98" s="7">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J98" s="7">
         <v>0</v>
@@ -4957,13 +5017,13 @@
         <v>215</v>
       </c>
       <c r="G99" s="3">
-        <v>950</v>
+        <v>1092</v>
       </c>
       <c r="H99" s="3">
         <v>0</v>
       </c>
       <c r="I99" s="3">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="J99" s="3">
         <v>0</v>
@@ -4986,13 +5046,13 @@
       <c r="E100" s="20"/>
       <c r="F100" s="8"/>
       <c r="G100" s="7">
-        <v>950</v>
+        <v>1092</v>
       </c>
       <c r="H100" s="7">
         <v>0</v>
       </c>
       <c r="I100" s="7">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="J100" s="7">
         <v>0</v>
@@ -5021,13 +5081,13 @@
         <v>218</v>
       </c>
       <c r="G101" s="3">
-        <v>938</v>
+        <v>1729</v>
       </c>
       <c r="H101" s="3">
         <v>0</v>
       </c>
       <c r="I101" s="3">
-        <v>133</v>
+        <v>244</v>
       </c>
       <c r="J101" s="3">
         <v>0</v>
@@ -5056,13 +5116,13 @@
         <v>220</v>
       </c>
       <c r="G102" s="3">
-        <v>1268</v>
+        <v>1431</v>
       </c>
       <c r="H102" s="3">
         <v>0</v>
       </c>
       <c r="I102" s="3">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="J102" s="3">
         <v>0</v>
@@ -5085,13 +5145,13 @@
       <c r="E103" s="20"/>
       <c r="F103" s="8"/>
       <c r="G103" s="7">
-        <v>2206</v>
+        <v>3160</v>
       </c>
       <c r="H103" s="7">
         <v>0</v>
       </c>
       <c r="I103" s="7">
-        <v>317</v>
+        <v>446</v>
       </c>
       <c r="J103" s="7">
         <v>0</v>
@@ -5123,13 +5183,13 @@
         <v>0</v>
       </c>
       <c r="H104" s="3">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I104" s="3">
         <v>0</v>
       </c>
       <c r="J104" s="3">
-        <v>240.27</v>
+        <v>259</v>
       </c>
       <c r="K104" s="3">
         <v>0</v>
@@ -5155,7 +5215,7 @@
         <v>226</v>
       </c>
       <c r="G105" s="3">
-        <v>669</v>
+        <v>1321</v>
       </c>
       <c r="H105" s="3">
         <v>0</v>
@@ -5164,7 +5224,7 @@
         <v>0</v>
       </c>
       <c r="J105" s="3">
-        <v>81.280000000000015</v>
+        <v>157.61</v>
       </c>
       <c r="K105" s="3">
         <v>0</v>
@@ -5190,7 +5250,7 @@
         <v>227</v>
       </c>
       <c r="G106" s="3">
-        <v>944</v>
+        <v>1465</v>
       </c>
       <c r="H106" s="3">
         <v>0</v>
@@ -5199,7 +5259,7 @@
         <v>0</v>
       </c>
       <c r="J106" s="3">
-        <v>112.54999999999998</v>
+        <v>172.49000000000004</v>
       </c>
       <c r="K106" s="3">
         <v>0</v>
@@ -5228,13 +5288,13 @@
         <v>0</v>
       </c>
       <c r="H107" s="3">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="I107" s="3">
         <v>0</v>
       </c>
       <c r="J107" s="3">
-        <v>304.96</v>
+        <v>460</v>
       </c>
       <c r="K107" s="3">
         <v>0</v>
@@ -5260,19 +5320,19 @@
         <v>232</v>
       </c>
       <c r="G108" s="3">
-        <v>228</v>
+        <v>295</v>
       </c>
       <c r="H108" s="3">
         <v>0</v>
       </c>
       <c r="I108" s="3">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J108" s="3">
         <v>0</v>
       </c>
       <c r="K108" s="3">
-        <v>53.260000000000005</v>
+        <v>69.039999999999992</v>
       </c>
     </row>
     <row r="109" hidden="1" outlineLevel="2">
@@ -5295,7 +5355,7 @@
         <v>233</v>
       </c>
       <c r="G109" s="3">
-        <v>309</v>
+        <v>611</v>
       </c>
       <c r="H109" s="3">
         <v>0</v>
@@ -5304,7 +5364,7 @@
         <v>0</v>
       </c>
       <c r="J109" s="3">
-        <v>69.389999999999986</v>
+        <v>132.83999999999998</v>
       </c>
       <c r="K109" s="3">
         <v>0</v>
@@ -5330,19 +5390,19 @@
         <v>235</v>
       </c>
       <c r="G110" s="3">
-        <v>409</v>
+        <v>1002</v>
       </c>
       <c r="H110" s="3">
         <v>0</v>
       </c>
       <c r="I110" s="3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J110" s="3">
         <v>0</v>
       </c>
       <c r="K110" s="3">
-        <v>87.74</v>
+        <v>208.21999999999997</v>
       </c>
     </row>
     <row r="111" hidden="1" outlineLevel="2">
@@ -5365,7 +5425,7 @@
         <v>236</v>
       </c>
       <c r="G111" s="3">
-        <v>271</v>
+        <v>322</v>
       </c>
       <c r="H111" s="3">
         <v>0</v>
@@ -5374,7 +5434,7 @@
         <v>0</v>
       </c>
       <c r="J111" s="3">
-        <v>60.86</v>
+        <v>70.100000000000009</v>
       </c>
       <c r="K111" s="3">
         <v>0</v>
@@ -5400,13 +5460,13 @@
         <v>237</v>
       </c>
       <c r="G112" s="3">
-        <v>393</v>
+        <v>728</v>
       </c>
       <c r="H112" s="3">
         <v>0</v>
       </c>
       <c r="I112" s="3">
-        <v>77.47999999999999</v>
+        <v>142.27999999999997</v>
       </c>
       <c r="J112" s="3">
         <v>0</v>
@@ -5435,19 +5495,19 @@
         <v>240</v>
       </c>
       <c r="G113" s="3">
-        <v>33</v>
+        <v>466</v>
       </c>
       <c r="H113" s="3">
         <v>0</v>
       </c>
       <c r="I113" s="3">
-        <v>6.73</v>
+        <v>18.98</v>
       </c>
       <c r="J113" s="3">
         <v>0</v>
       </c>
       <c r="K113" s="3">
-        <v>28</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="114" hidden="1" outlineLevel="2">
@@ -5470,13 +5530,13 @@
         <v>243</v>
       </c>
       <c r="G114" s="3">
-        <v>250</v>
+        <v>661</v>
       </c>
       <c r="H114" s="3">
         <v>0</v>
       </c>
       <c r="I114" s="3">
-        <v>28.97</v>
+        <v>73.679999999999993</v>
       </c>
       <c r="J114" s="3">
         <v>0</v>
@@ -5505,13 +5565,13 @@
         <v>244</v>
       </c>
       <c r="G115" s="3">
-        <v>1014</v>
+        <v>475</v>
       </c>
       <c r="H115" s="3">
         <v>0</v>
       </c>
       <c r="I115" s="3">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="J115" s="3">
         <v>0</v>
@@ -5540,19 +5600,19 @@
         <v>246</v>
       </c>
       <c r="G116" s="3">
-        <v>234</v>
+        <v>724</v>
       </c>
       <c r="H116" s="3">
         <v>0</v>
       </c>
       <c r="I116" s="3">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J116" s="3">
         <v>0</v>
       </c>
       <c r="K116" s="3">
-        <v>50.669999999999995</v>
+        <v>168.85</v>
       </c>
     </row>
     <row r="117" hidden="1" outlineLevel="1" collapsed="1" s="7" customFormat="1">
@@ -5569,19 +5629,19 @@
       <c r="E117" s="8"/>
       <c r="F117" s="8"/>
       <c r="G117" s="7">
-        <v>4754</v>
+        <v>8070</v>
       </c>
       <c r="H117" s="7">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="I117" s="7">
-        <v>246.18</v>
+        <v>328.93999999999994</v>
       </c>
       <c r="J117" s="7">
-        <v>869.31</v>
+        <v>1252.0399999999997</v>
       </c>
       <c r="K117" s="7">
-        <v>219.67</v>
+        <v>539.61</v>
       </c>
     </row>
     <row r="118" hidden="1" outlineLevel="2">
@@ -5623,21 +5683,6 @@
       <c r="F119" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="G119" s="3">
-        <v>2576</v>
-      </c>
-      <c r="H119" s="3">
-        <v>0</v>
-      </c>
-      <c r="I119" s="3">
-        <v>0</v>
-      </c>
-      <c r="J119" s="3">
-        <v>303</v>
-      </c>
-      <c r="K119" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="120" hidden="1" outlineLevel="2">
       <c r="A120" s="16">
@@ -5659,13 +5704,13 @@
         <v>251</v>
       </c>
       <c r="G120" s="3">
-        <v>942</v>
+        <v>1008</v>
       </c>
       <c r="H120" s="3">
         <v>0</v>
       </c>
       <c r="I120" s="3">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="J120" s="3">
         <v>0</v>
@@ -5693,21 +5738,6 @@
       <c r="F121" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="G121" s="3">
-        <v>0</v>
-      </c>
-      <c r="H121" s="3">
-        <v>46</v>
-      </c>
-      <c r="I121" s="3">
-        <v>0</v>
-      </c>
-      <c r="J121" s="3">
-        <v>285</v>
-      </c>
-      <c r="K121" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="122" hidden="1" outlineLevel="2">
       <c r="A122" s="16">
@@ -5729,7 +5759,7 @@
         <v>254</v>
       </c>
       <c r="G122" s="3">
-        <v>575</v>
+        <v>435</v>
       </c>
       <c r="H122" s="3">
         <v>0</v>
@@ -5738,7 +5768,7 @@
         <v>0</v>
       </c>
       <c r="J122" s="3">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="K122" s="3">
         <v>0</v>
@@ -5764,7 +5794,7 @@
         <v>255</v>
       </c>
       <c r="G123" s="3">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="H123" s="3">
         <v>0</v>
@@ -5773,7 +5803,7 @@
         <v>0</v>
       </c>
       <c r="J123" s="3">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K123" s="3">
         <v>0</v>
@@ -5799,13 +5829,13 @@
         <v>256</v>
       </c>
       <c r="G124" s="3">
-        <v>393</v>
+        <v>721</v>
       </c>
       <c r="H124" s="3">
         <v>0</v>
       </c>
       <c r="I124" s="3">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="J124" s="3">
         <v>0</v>
@@ -5834,7 +5864,7 @@
         <v>257</v>
       </c>
       <c r="G125" s="3">
-        <v>109</v>
+        <v>612</v>
       </c>
       <c r="H125" s="3">
         <v>0</v>
@@ -5843,7 +5873,7 @@
         <v>0</v>
       </c>
       <c r="J125" s="3">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="K125" s="3">
         <v>0</v>
@@ -5869,7 +5899,7 @@
         <v>259</v>
       </c>
       <c r="G126" s="3">
-        <v>54</v>
+        <v>582</v>
       </c>
       <c r="H126" s="3">
         <v>0</v>
@@ -5878,7 +5908,7 @@
         <v>0</v>
       </c>
       <c r="J126" s="3">
-        <v>26</v>
+        <v>191</v>
       </c>
       <c r="K126" s="3">
         <v>0</v>
@@ -5904,19 +5934,19 @@
         <v>260</v>
       </c>
       <c r="G127" s="3">
-        <v>755</v>
+        <v>596</v>
       </c>
       <c r="H127" s="3">
         <v>0</v>
       </c>
       <c r="I127" s="3">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="J127" s="3">
         <v>0</v>
       </c>
       <c r="K127" s="3">
-        <v>217</v>
+        <v>142</v>
       </c>
     </row>
     <row r="128" hidden="1" outlineLevel="2">
@@ -5939,7 +5969,7 @@
         <v>261</v>
       </c>
       <c r="G128" s="3">
-        <v>2649</v>
+        <v>2458</v>
       </c>
       <c r="H128" s="3">
         <v>0</v>
@@ -5948,7 +5978,7 @@
         <v>0</v>
       </c>
       <c r="J128" s="3">
-        <v>326</v>
+        <v>290</v>
       </c>
       <c r="K128" s="3">
         <v>0</v>
@@ -5974,13 +6004,13 @@
         <v>262</v>
       </c>
       <c r="G129" s="3">
-        <v>1357</v>
+        <v>1076</v>
       </c>
       <c r="H129" s="3">
         <v>0</v>
       </c>
       <c r="I129" s="3">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="J129" s="3">
         <v>0</v>
@@ -6009,19 +6039,19 @@
         <v>263</v>
       </c>
       <c r="G130" s="3">
-        <v>524</v>
+        <v>409</v>
       </c>
       <c r="H130" s="3">
         <v>0</v>
       </c>
       <c r="I130" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J130" s="3">
         <v>0</v>
       </c>
       <c r="K130" s="3">
-        <v>153</v>
+        <v>99</v>
       </c>
     </row>
     <row r="131" hidden="1" outlineLevel="1" collapsed="1" s="7" customFormat="1">
@@ -6038,19 +6068,19 @@
       <c r="E131" s="8"/>
       <c r="F131" s="8"/>
       <c r="G131" s="7">
-        <v>9934</v>
+        <v>8167</v>
       </c>
       <c r="H131" s="7">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="I131" s="7">
-        <v>377</v>
+        <v>397</v>
       </c>
       <c r="J131" s="7">
-        <v>1055</v>
+        <v>741</v>
       </c>
       <c r="K131" s="7">
-        <v>370</v>
+        <v>241</v>
       </c>
     </row>
     <row r="132" hidden="1" outlineLevel="2">
@@ -6076,13 +6106,13 @@
         <v>0</v>
       </c>
       <c r="H132" s="3">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="I132" s="3">
         <v>0</v>
       </c>
       <c r="J132" s="3">
-        <v>235</v>
+        <v>503</v>
       </c>
       <c r="K132" s="3">
         <v>0</v>
@@ -6108,7 +6138,7 @@
         <v>267</v>
       </c>
       <c r="G133" s="3">
-        <v>153</v>
+        <v>1664</v>
       </c>
       <c r="H133" s="3">
         <v>0</v>
@@ -6117,7 +6147,7 @@
         <v>0</v>
       </c>
       <c r="J133" s="3">
-        <v>50</v>
+        <v>535</v>
       </c>
       <c r="K133" s="3">
         <v>0</v>
@@ -6143,19 +6173,19 @@
         <v>268</v>
       </c>
       <c r="G134" s="3">
-        <v>0</v>
+        <v>511</v>
       </c>
       <c r="H134" s="3">
         <v>0</v>
       </c>
       <c r="I134" s="3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J134" s="3">
         <v>0</v>
       </c>
       <c r="K134" s="3">
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
     <row r="135" hidden="1" outlineLevel="2">
@@ -6178,13 +6208,13 @@
         <v>269</v>
       </c>
       <c r="G135" s="3">
-        <v>59</v>
+        <v>604</v>
       </c>
       <c r="H135" s="3">
         <v>0</v>
       </c>
       <c r="I135" s="3">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="J135" s="3">
         <v>0</v>
@@ -6213,7 +6243,7 @@
         <v>270</v>
       </c>
       <c r="G136" s="3">
-        <v>1925</v>
+        <v>2426</v>
       </c>
       <c r="H136" s="3">
         <v>0</v>
@@ -6222,7 +6252,7 @@
         <v>0</v>
       </c>
       <c r="J136" s="3">
-        <v>231</v>
+        <v>279</v>
       </c>
       <c r="K136" s="3">
         <v>0</v>
@@ -6248,7 +6278,7 @@
         <v>271</v>
       </c>
       <c r="G137" s="3">
-        <v>3227</v>
+        <v>2260</v>
       </c>
       <c r="H137" s="3">
         <v>0</v>
@@ -6257,7 +6287,7 @@
         <v>0</v>
       </c>
       <c r="J137" s="3">
-        <v>387</v>
+        <v>259</v>
       </c>
       <c r="K137" s="3">
         <v>0</v>
@@ -6283,13 +6313,13 @@
         <v>272</v>
       </c>
       <c r="G138" s="3">
-        <v>0</v>
+        <v>618</v>
       </c>
       <c r="H138" s="3">
         <v>0</v>
       </c>
       <c r="I138" s="3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="J138" s="3">
         <v>0</v>
@@ -6318,7 +6348,7 @@
         <v>273</v>
       </c>
       <c r="G139" s="3">
-        <v>127</v>
+        <v>496</v>
       </c>
       <c r="H139" s="3">
         <v>0</v>
@@ -6327,7 +6357,7 @@
         <v>0</v>
       </c>
       <c r="J139" s="3">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="K139" s="3">
         <v>0</v>
@@ -6353,7 +6383,7 @@
         <v>275</v>
       </c>
       <c r="G140" s="3">
-        <v>102</v>
+        <v>387</v>
       </c>
       <c r="H140" s="3">
         <v>0</v>
@@ -6362,7 +6392,7 @@
         <v>0</v>
       </c>
       <c r="J140" s="3">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="K140" s="3">
         <v>0</v>
@@ -6388,7 +6418,7 @@
         <v>276</v>
       </c>
       <c r="G141" s="3">
-        <v>0</v>
+        <v>334</v>
       </c>
       <c r="H141" s="3">
         <v>0</v>
@@ -6397,7 +6427,7 @@
         <v>0</v>
       </c>
       <c r="J141" s="3">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="K141" s="3">
         <v>0</v>
@@ -6423,7 +6453,7 @@
         <v>277</v>
       </c>
       <c r="G142" s="3">
-        <v>1288</v>
+        <v>532</v>
       </c>
       <c r="H142" s="3">
         <v>0</v>
@@ -6432,7 +6462,7 @@
         <v>0</v>
       </c>
       <c r="J142" s="3">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="K142" s="3">
         <v>0</v>
@@ -6458,7 +6488,7 @@
         <v>278</v>
       </c>
       <c r="G143" s="3">
-        <v>0</v>
+        <v>809</v>
       </c>
       <c r="H143" s="3">
         <v>0</v>
@@ -6467,7 +6497,7 @@
         <v>0</v>
       </c>
       <c r="J143" s="3">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="K143" s="3">
         <v>0</v>
@@ -6487,19 +6517,19 @@
       <c r="E144" s="8"/>
       <c r="F144" s="8"/>
       <c r="G144" s="7">
-        <v>6881</v>
+        <v>10641</v>
       </c>
       <c r="H144" s="7">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="I144" s="7">
-        <v>11</v>
+        <v>331</v>
       </c>
       <c r="J144" s="7">
-        <v>1049</v>
+        <v>1924</v>
       </c>
       <c r="K144" s="7">
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
     <row r="145" hidden="1" outlineLevel="2">
@@ -6521,21 +6551,6 @@
       <c r="F145" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="G145" s="3">
-        <v>0</v>
-      </c>
-      <c r="H145" s="3">
-        <v>78</v>
-      </c>
-      <c r="I145" s="3">
-        <v>0</v>
-      </c>
-      <c r="J145" s="3">
-        <v>416</v>
-      </c>
-      <c r="K145" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="146" hidden="1" outlineLevel="2">
       <c r="A146" s="16">
@@ -6557,7 +6572,7 @@
         <v>281</v>
       </c>
       <c r="G146" s="3">
-        <v>0</v>
+        <v>961</v>
       </c>
       <c r="H146" s="3">
         <v>0</v>
@@ -6566,7 +6581,7 @@
         <v>0</v>
       </c>
       <c r="J146" s="3">
-        <v>0</v>
+        <v>314</v>
       </c>
       <c r="K146" s="3">
         <v>0</v>
@@ -6592,7 +6607,7 @@
         <v>282</v>
       </c>
       <c r="G147" s="3">
-        <v>1153</v>
+        <v>2543</v>
       </c>
       <c r="H147" s="3">
         <v>0</v>
@@ -6601,7 +6616,7 @@
         <v>0</v>
       </c>
       <c r="J147" s="3">
-        <v>212</v>
+        <v>467</v>
       </c>
       <c r="K147" s="3">
         <v>0</v>
@@ -6627,7 +6642,7 @@
         <v>283</v>
       </c>
       <c r="G148" s="3">
-        <v>1354</v>
+        <v>3027</v>
       </c>
       <c r="H148" s="3">
         <v>0</v>
@@ -6636,7 +6651,7 @@
         <v>0</v>
       </c>
       <c r="J148" s="3">
-        <v>249</v>
+        <v>551</v>
       </c>
       <c r="K148" s="3">
         <v>0</v>
@@ -6662,7 +6677,7 @@
         <v>285</v>
       </c>
       <c r="G149" s="3">
-        <v>128</v>
+        <v>351</v>
       </c>
       <c r="H149" s="3">
         <v>0</v>
@@ -6671,7 +6686,7 @@
         <v>0</v>
       </c>
       <c r="J149" s="3">
-        <v>43</v>
+        <v>157</v>
       </c>
       <c r="K149" s="3">
         <v>0</v>
@@ -6697,7 +6712,7 @@
         <v>286</v>
       </c>
       <c r="G150" s="3">
-        <v>15</v>
+        <v>789</v>
       </c>
       <c r="H150" s="3">
         <v>0</v>
@@ -6706,7 +6721,7 @@
         <v>0</v>
       </c>
       <c r="J150" s="3">
-        <v>7</v>
+        <v>347</v>
       </c>
       <c r="K150" s="3">
         <v>0</v>
@@ -6732,13 +6747,13 @@
         <v>288</v>
       </c>
       <c r="G151" s="3">
-        <v>574</v>
+        <v>770</v>
       </c>
       <c r="H151" s="3">
         <v>0</v>
       </c>
       <c r="I151" s="3">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="J151" s="3">
         <v>0</v>
@@ -6767,7 +6782,7 @@
         <v>289</v>
       </c>
       <c r="G152" s="3">
-        <v>138</v>
+        <v>504</v>
       </c>
       <c r="H152" s="3">
         <v>0</v>
@@ -6776,7 +6791,7 @@
         <v>0</v>
       </c>
       <c r="J152" s="3">
-        <v>55</v>
+        <v>225</v>
       </c>
       <c r="K152" s="3">
         <v>0</v>
@@ -6802,19 +6817,19 @@
         <v>290</v>
       </c>
       <c r="G153" s="3">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="H153" s="3">
         <v>0</v>
       </c>
       <c r="I153" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J153" s="3">
         <v>0</v>
       </c>
       <c r="K153" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154" hidden="1" outlineLevel="2">
@@ -6837,13 +6852,13 @@
         <v>292</v>
       </c>
       <c r="G154" s="3">
-        <v>217</v>
+        <v>732</v>
       </c>
       <c r="H154" s="3">
         <v>0</v>
       </c>
       <c r="I154" s="3">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="J154" s="3">
         <v>0</v>
@@ -6872,19 +6887,19 @@
         <v>294</v>
       </c>
       <c r="G155" s="3">
-        <v>259</v>
+        <v>888</v>
       </c>
       <c r="H155" s="3">
         <v>0</v>
       </c>
       <c r="I155" s="3">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="J155" s="3">
         <v>0</v>
       </c>
       <c r="K155" s="3">
-        <v>97</v>
+        <v>370</v>
       </c>
     </row>
     <row r="156" hidden="1" outlineLevel="1" collapsed="1" s="7" customFormat="1">
@@ -6901,19 +6916,19 @@
       <c r="E156" s="8"/>
       <c r="F156" s="8"/>
       <c r="G156" s="7">
-        <v>3861</v>
+        <v>10578</v>
       </c>
       <c r="H156" s="7">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="I156" s="7">
-        <v>237</v>
+        <v>429</v>
       </c>
       <c r="J156" s="7">
-        <v>982</v>
+        <v>2061</v>
       </c>
       <c r="K156" s="7">
-        <v>104</v>
+        <v>374</v>
       </c>
     </row>
     <row r="157" hidden="1" outlineLevel="2">
@@ -6939,13 +6954,13 @@
         <v>0</v>
       </c>
       <c r="H157" s="3">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="I157" s="3">
         <v>0</v>
       </c>
       <c r="J157" s="3">
-        <v>90</v>
+        <v>300</v>
       </c>
       <c r="K157" s="3">
         <v>0</v>
@@ -6970,6 +6985,21 @@
       <c r="F158" s="14" t="s">
         <v>297</v>
       </c>
+      <c r="G158" s="3">
+        <v>286</v>
+      </c>
+      <c r="H158" s="3">
+        <v>0</v>
+      </c>
+      <c r="I158" s="3">
+        <v>0</v>
+      </c>
+      <c r="J158" s="3">
+        <v>73</v>
+      </c>
+      <c r="K158" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="159" hidden="1" outlineLevel="2">
       <c r="A159" s="16">
@@ -7010,6 +7040,21 @@
       <c r="F160" s="14" t="s">
         <v>299</v>
       </c>
+      <c r="G160" s="3">
+        <v>415</v>
+      </c>
+      <c r="H160" s="3">
+        <v>0</v>
+      </c>
+      <c r="I160" s="3">
+        <v>14</v>
+      </c>
+      <c r="J160" s="3">
+        <v>0</v>
+      </c>
+      <c r="K160" s="3">
+        <v>104</v>
+      </c>
     </row>
     <row r="161" hidden="1" outlineLevel="2">
       <c r="A161" s="16">
@@ -7031,7 +7076,7 @@
         <v>300</v>
       </c>
       <c r="G161" s="3">
-        <v>1603</v>
+        <v>1591</v>
       </c>
       <c r="H161" s="3">
         <v>0</v>
@@ -7040,7 +7085,7 @@
         <v>0</v>
       </c>
       <c r="J161" s="3">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="K161" s="3">
         <v>0</v>
@@ -7066,7 +7111,7 @@
         <v>301</v>
       </c>
       <c r="G162" s="3">
-        <v>1577</v>
+        <v>1523</v>
       </c>
       <c r="H162" s="3">
         <v>0</v>
@@ -7075,7 +7120,7 @@
         <v>0</v>
       </c>
       <c r="J162" s="3">
-        <v>207</v>
+        <v>237</v>
       </c>
       <c r="K162" s="3">
         <v>0</v>
@@ -7101,19 +7146,19 @@
         <v>302</v>
       </c>
       <c r="G163" s="3">
-        <v>20</v>
+        <v>850</v>
       </c>
       <c r="H163" s="3">
         <v>0</v>
       </c>
       <c r="I163" s="3">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="J163" s="3">
         <v>0</v>
       </c>
       <c r="K163" s="3">
-        <v>6</v>
+        <v>194</v>
       </c>
     </row>
     <row r="164" hidden="1" outlineLevel="2">
@@ -7156,7 +7201,7 @@
         <v>304</v>
       </c>
       <c r="G165" s="3">
-        <v>49</v>
+        <v>303</v>
       </c>
       <c r="H165" s="3">
         <v>0</v>
@@ -7165,7 +7210,7 @@
         <v>0</v>
       </c>
       <c r="J165" s="3">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="K165" s="3">
         <v>0</v>
@@ -7191,7 +7236,7 @@
         <v>306</v>
       </c>
       <c r="G166" s="3">
-        <v>763</v>
+        <v>639</v>
       </c>
       <c r="H166" s="3">
         <v>0</v>
@@ -7200,7 +7245,7 @@
         <v>0</v>
       </c>
       <c r="J166" s="3">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="K166" s="3">
         <v>0</v>
@@ -7226,13 +7271,13 @@
         <v>307</v>
       </c>
       <c r="G167" s="3">
-        <v>327</v>
+        <v>961</v>
       </c>
       <c r="H167" s="3">
         <v>0</v>
       </c>
       <c r="I167" s="3">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="J167" s="3">
         <v>0</v>
@@ -7261,13 +7306,13 @@
         <v>308</v>
       </c>
       <c r="G168" s="3">
-        <v>229</v>
+        <v>100</v>
       </c>
       <c r="H168" s="3">
         <v>0</v>
       </c>
       <c r="I168" s="3">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="J168" s="3">
         <v>0</v>
@@ -7290,19 +7335,19 @@
       <c r="E169" s="8"/>
       <c r="F169" s="8"/>
       <c r="G169" s="7">
-        <v>4568</v>
+        <v>6668</v>
       </c>
       <c r="H169" s="7">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="I169" s="7">
-        <v>56</v>
+        <v>132</v>
       </c>
       <c r="J169" s="7">
-        <v>650</v>
+        <v>992</v>
       </c>
       <c r="K169" s="7">
-        <v>6</v>
+        <v>298</v>
       </c>
     </row>
     <row r="170" hidden="1" outlineLevel="2">
@@ -7328,13 +7373,13 @@
         <v>0</v>
       </c>
       <c r="H170" s="3">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="I170" s="3">
         <v>0</v>
       </c>
       <c r="J170" s="3">
-        <v>584</v>
+        <v>612</v>
       </c>
       <c r="K170" s="3">
         <v>0</v>
@@ -7359,21 +7404,6 @@
       <c r="F171" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="G171" s="3">
-        <v>120</v>
-      </c>
-      <c r="H171" s="3">
-        <v>0</v>
-      </c>
-      <c r="I171" s="3">
-        <v>39</v>
-      </c>
-      <c r="J171" s="3">
-        <v>0</v>
-      </c>
-      <c r="K171" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="172" hidden="1" outlineLevel="2">
       <c r="A172" s="16">
@@ -7395,19 +7425,19 @@
         <v>314</v>
       </c>
       <c r="G172" s="3">
-        <v>0</v>
+        <v>971</v>
       </c>
       <c r="H172" s="3">
         <v>0</v>
       </c>
       <c r="I172" s="3">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J172" s="3">
         <v>0</v>
       </c>
       <c r="K172" s="3">
-        <v>0</v>
+        <v>195</v>
       </c>
     </row>
     <row r="173" hidden="1" outlineLevel="2">
@@ -7430,7 +7460,7 @@
         <v>315</v>
       </c>
       <c r="G173" s="3">
-        <v>1500</v>
+        <v>2765</v>
       </c>
       <c r="H173" s="3">
         <v>0</v>
@@ -7439,7 +7469,7 @@
         <v>0</v>
       </c>
       <c r="J173" s="3">
-        <v>174</v>
+        <v>280</v>
       </c>
       <c r="K173" s="3">
         <v>0</v>
@@ -7465,7 +7495,7 @@
         <v>316</v>
       </c>
       <c r="G174" s="3">
-        <v>2352</v>
+        <v>3886</v>
       </c>
       <c r="H174" s="3">
         <v>0</v>
@@ -7474,7 +7504,7 @@
         <v>0</v>
       </c>
       <c r="J174" s="3">
-        <v>251</v>
+        <v>436</v>
       </c>
       <c r="K174" s="3">
         <v>0</v>
@@ -7503,13 +7533,13 @@
         <v>0</v>
       </c>
       <c r="H175" s="3">
-        <v>67</v>
+        <v>55.5</v>
       </c>
       <c r="I175" s="3">
         <v>0</v>
       </c>
       <c r="J175" s="3">
-        <v>380</v>
+        <v>321</v>
       </c>
       <c r="K175" s="3">
         <v>0</v>
@@ -7535,13 +7565,13 @@
         <v>318</v>
       </c>
       <c r="G176" s="3">
-        <v>258</v>
+        <v>1604</v>
       </c>
       <c r="H176" s="3">
         <v>0</v>
       </c>
       <c r="I176" s="3">
-        <v>50</v>
+        <v>304</v>
       </c>
       <c r="J176" s="3">
         <v>0</v>
@@ -7570,7 +7600,7 @@
         <v>319</v>
       </c>
       <c r="G177" s="3">
-        <v>96</v>
+        <v>718</v>
       </c>
       <c r="H177" s="3">
         <v>0</v>
@@ -7579,7 +7609,7 @@
         <v>0</v>
       </c>
       <c r="J177" s="3">
-        <v>32</v>
+        <v>237</v>
       </c>
       <c r="K177" s="3">
         <v>0</v>
@@ -7605,7 +7635,7 @@
         <v>320</v>
       </c>
       <c r="G178" s="3">
-        <v>125</v>
+        <v>596</v>
       </c>
       <c r="H178" s="3">
         <v>0</v>
@@ -7614,7 +7644,7 @@
         <v>0</v>
       </c>
       <c r="J178" s="3">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="K178" s="3">
         <v>0</v>
@@ -7640,7 +7670,7 @@
         <v>321</v>
       </c>
       <c r="G179" s="3">
-        <v>100</v>
+        <v>603</v>
       </c>
       <c r="H179" s="3">
         <v>0</v>
@@ -7649,7 +7679,7 @@
         <v>0</v>
       </c>
       <c r="J179" s="3">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="K179" s="3">
         <v>0</v>
@@ -7675,7 +7705,7 @@
         <v>322</v>
       </c>
       <c r="G180" s="3">
-        <v>161</v>
+        <v>225</v>
       </c>
       <c r="H180" s="3">
         <v>0</v>
@@ -7684,7 +7714,7 @@
         <v>0</v>
       </c>
       <c r="J180" s="3">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="K180" s="3">
         <v>0</v>
@@ -7710,13 +7740,13 @@
         <v>323</v>
       </c>
       <c r="G181" s="3">
-        <v>411</v>
+        <v>823</v>
       </c>
       <c r="H181" s="3">
         <v>0</v>
       </c>
       <c r="I181" s="3">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="J181" s="3">
         <v>0</v>
@@ -7745,19 +7775,19 @@
         <v>324</v>
       </c>
       <c r="G182" s="3">
-        <v>371</v>
+        <v>316</v>
       </c>
       <c r="H182" s="3">
         <v>0</v>
       </c>
       <c r="I182" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J182" s="3">
         <v>0</v>
       </c>
       <c r="K182" s="3">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="183" hidden="1" outlineLevel="2">
@@ -7780,19 +7810,19 @@
         <v>325</v>
       </c>
       <c r="G183" s="3">
-        <v>384</v>
+        <v>863</v>
       </c>
       <c r="H183" s="3">
         <v>0</v>
       </c>
       <c r="I183" s="3">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J183" s="3">
         <v>0</v>
       </c>
       <c r="K183" s="3">
-        <v>67</v>
+        <v>181</v>
       </c>
     </row>
     <row r="184" hidden="1" outlineLevel="2">
@@ -7815,13 +7845,13 @@
         <v>326</v>
       </c>
       <c r="G184" s="3">
-        <v>352</v>
+        <v>388</v>
       </c>
       <c r="H184" s="3">
         <v>0</v>
       </c>
       <c r="I184" s="3">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J184" s="3">
         <v>0</v>
@@ -7844,19 +7874,19 @@
       <c r="E185" s="8"/>
       <c r="F185" s="8"/>
       <c r="G185" s="7">
-        <v>6230</v>
+        <v>13758</v>
       </c>
       <c r="H185" s="7">
-        <v>186</v>
+        <v>178.5</v>
       </c>
       <c r="I185" s="7">
-        <v>216</v>
+        <v>520</v>
       </c>
       <c r="J185" s="7">
-        <v>1507</v>
+        <v>2197</v>
       </c>
       <c r="K185" s="7">
-        <v>145</v>
+        <v>442</v>
       </c>
     </row>
     <row r="186" hidden="1" outlineLevel="2">
@@ -7879,13 +7909,13 @@
         <v>329</v>
       </c>
       <c r="G186" s="3">
-        <v>1410</v>
+        <v>1450</v>
       </c>
       <c r="H186" s="3">
         <v>0</v>
       </c>
       <c r="I186" s="3">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J186" s="3">
         <v>0</v>
@@ -7914,19 +7944,19 @@
         <v>332</v>
       </c>
       <c r="G187" s="3">
-        <v>1086</v>
+        <v>714</v>
       </c>
       <c r="H187" s="3">
         <v>0</v>
       </c>
       <c r="I187" s="3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J187" s="3">
         <v>0</v>
       </c>
       <c r="K187" s="3">
-        <v>129</v>
+        <v>82</v>
       </c>
     </row>
     <row r="188" hidden="1" outlineLevel="1" collapsed="1" s="7" customFormat="1">
@@ -7943,19 +7973,19 @@
       <c r="E188" s="8"/>
       <c r="F188" s="8"/>
       <c r="G188" s="7">
-        <v>2496</v>
+        <v>2164</v>
       </c>
       <c r="H188" s="7">
         <v>0</v>
       </c>
       <c r="I188" s="7">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="J188" s="7">
         <v>0</v>
       </c>
       <c r="K188" s="7">
-        <v>129</v>
+        <v>82</v>
       </c>
     </row>
     <row r="189" hidden="1" outlineLevel="2">
@@ -7977,6 +8007,21 @@
       <c r="F189" s="14" t="s">
         <v>334</v>
       </c>
+      <c r="G189" s="3">
+        <v>1009</v>
+      </c>
+      <c r="H189" s="3">
+        <v>0</v>
+      </c>
+      <c r="I189" s="3">
+        <v>0</v>
+      </c>
+      <c r="J189" s="3">
+        <v>93</v>
+      </c>
+      <c r="K189" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="190" hidden="1" outlineLevel="2">
       <c r="A190" s="16">
@@ -7997,21 +8042,6 @@
       <c r="F190" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="G190" s="3">
-        <v>0</v>
-      </c>
-      <c r="H190" s="3">
-        <v>11.000000000000002</v>
-      </c>
-      <c r="I190" s="3">
-        <v>91</v>
-      </c>
-      <c r="J190" s="3">
-        <v>0</v>
-      </c>
-      <c r="K190" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="191" hidden="1" outlineLevel="2">
       <c r="A191" s="16">
@@ -8036,13 +8066,13 @@
         <v>0</v>
       </c>
       <c r="H191" s="3">
-        <v>10.400000000000002</v>
+        <v>19.900000000000006</v>
       </c>
       <c r="I191" s="3">
         <v>0</v>
       </c>
       <c r="J191" s="3">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="K191" s="3">
         <v>0</v>
@@ -8062,16 +8092,16 @@
       <c r="E192" s="8"/>
       <c r="F192" s="8"/>
       <c r="G192" s="7">
-        <v>0</v>
+        <v>1009</v>
       </c>
       <c r="H192" s="7">
-        <v>21.400000000000006</v>
+        <v>19.900000000000006</v>
       </c>
       <c r="I192" s="7">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="J192" s="7">
-        <v>51</v>
+        <v>186</v>
       </c>
       <c r="K192" s="7">
         <v>0</v>
@@ -8097,13 +8127,13 @@
         <v>342</v>
       </c>
       <c r="G193" s="3">
-        <v>821</v>
+        <v>682</v>
       </c>
       <c r="H193" s="3">
         <v>0</v>
       </c>
       <c r="I193" s="3">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="J193" s="3">
         <v>0</v>
@@ -8132,19 +8162,19 @@
         <v>344</v>
       </c>
       <c r="G194" s="3">
-        <v>709</v>
+        <v>264</v>
       </c>
       <c r="H194" s="3">
         <v>0</v>
       </c>
       <c r="I194" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J194" s="3">
         <v>0</v>
       </c>
       <c r="K194" s="3">
-        <v>88</v>
+        <v>32</v>
       </c>
     </row>
     <row r="195" hidden="1" outlineLevel="2">
@@ -8167,19 +8197,19 @@
         <v>345</v>
       </c>
       <c r="G195" s="3">
-        <v>1557</v>
+        <v>1440</v>
       </c>
       <c r="H195" s="3">
         <v>0</v>
       </c>
       <c r="I195" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J195" s="3">
         <v>0</v>
       </c>
       <c r="K195" s="3">
-        <v>337</v>
+        <v>309</v>
       </c>
     </row>
     <row r="196" hidden="1" outlineLevel="2">
@@ -8202,7 +8232,7 @@
         <v>347</v>
       </c>
       <c r="G196" s="3">
-        <v>135</v>
+        <v>858</v>
       </c>
       <c r="H196" s="3">
         <v>0</v>
@@ -8211,7 +8241,7 @@
         <v>0</v>
       </c>
       <c r="J196" s="3">
-        <v>48</v>
+        <v>190</v>
       </c>
       <c r="K196" s="3">
         <v>0</v>
@@ -8237,7 +8267,7 @@
         <v>348</v>
       </c>
       <c r="G197" s="3">
-        <v>0</v>
+        <v>1458</v>
       </c>
       <c r="H197" s="3">
         <v>0</v>
@@ -8246,7 +8276,7 @@
         <v>0</v>
       </c>
       <c r="J197" s="3">
-        <v>0</v>
+        <v>318</v>
       </c>
       <c r="K197" s="3">
         <v>0</v>
@@ -8271,6 +8301,21 @@
       <c r="F198" s="14" t="s">
         <v>349</v>
       </c>
+      <c r="G198" s="3">
+        <v>901</v>
+      </c>
+      <c r="H198" s="3">
+        <v>0</v>
+      </c>
+      <c r="I198" s="3">
+        <v>0</v>
+      </c>
+      <c r="J198" s="3">
+        <v>199</v>
+      </c>
+      <c r="K198" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="199" hidden="1" outlineLevel="2">
       <c r="A199" s="16">
@@ -8292,7 +8337,7 @@
         <v>350</v>
       </c>
       <c r="G199" s="3">
-        <v>69</v>
+        <v>700</v>
       </c>
       <c r="H199" s="3">
         <v>0</v>
@@ -8301,7 +8346,7 @@
         <v>0</v>
       </c>
       <c r="J199" s="3">
-        <v>30</v>
+        <v>305</v>
       </c>
       <c r="K199" s="3">
         <v>0</v>
@@ -8327,7 +8372,7 @@
         <v>351</v>
       </c>
       <c r="G200" s="3">
-        <v>576</v>
+        <v>122</v>
       </c>
       <c r="H200" s="3">
         <v>0</v>
@@ -8336,7 +8381,7 @@
         <v>0</v>
       </c>
       <c r="J200" s="3">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="K200" s="3">
         <v>0</v>
@@ -8365,13 +8410,13 @@
         <v>0</v>
       </c>
       <c r="H201" s="3">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="I201" s="3">
         <v>0</v>
       </c>
       <c r="J201" s="3">
-        <v>971</v>
+        <v>1149</v>
       </c>
       <c r="K201" s="3">
         <v>0</v>
@@ -8396,21 +8441,6 @@
       <c r="F202" s="14" t="s">
         <v>355</v>
       </c>
-      <c r="G202" s="3">
-        <v>164</v>
-      </c>
-      <c r="H202" s="3">
-        <v>33.2</v>
-      </c>
-      <c r="I202" s="3">
-        <v>100</v>
-      </c>
-      <c r="J202" s="3">
-        <v>1407</v>
-      </c>
-      <c r="K202" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="203" hidden="1" outlineLevel="2">
       <c r="A203" s="16">
@@ -8432,16 +8462,16 @@
         <v>357</v>
       </c>
       <c r="G203" s="3">
-        <v>187</v>
+        <v>30</v>
       </c>
       <c r="H203" s="3">
-        <v>32.800000000000011</v>
+        <v>3</v>
       </c>
       <c r="I203" s="3">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="J203" s="3">
-        <v>1392</v>
+        <v>131</v>
       </c>
       <c r="K203" s="3">
         <v>0</v>
@@ -8467,7 +8497,7 @@
         <v>360</v>
       </c>
       <c r="G204" s="3">
-        <v>0</v>
+        <v>2660</v>
       </c>
       <c r="H204" s="3">
         <v>0</v>
@@ -8476,7 +8506,7 @@
         <v>0</v>
       </c>
       <c r="J204" s="3">
-        <v>0</v>
+        <v>791</v>
       </c>
       <c r="K204" s="3">
         <v>0</v>
@@ -8502,7 +8532,7 @@
         <v>362</v>
       </c>
       <c r="G205" s="3">
-        <v>0</v>
+        <v>2759</v>
       </c>
       <c r="H205" s="3">
         <v>0</v>
@@ -8511,7 +8541,7 @@
         <v>0</v>
       </c>
       <c r="J205" s="3">
-        <v>0</v>
+        <v>371</v>
       </c>
       <c r="K205" s="3">
         <v>0</v>
@@ -8577,7 +8607,7 @@
         <v>367</v>
       </c>
       <c r="G208" s="3">
-        <v>280</v>
+        <v>597</v>
       </c>
       <c r="H208" s="3">
         <v>0</v>
@@ -8586,7 +8616,7 @@
         <v>0</v>
       </c>
       <c r="J208" s="3">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="K208" s="3">
         <v>0</v>
@@ -8611,6 +8641,21 @@
       <c r="F209" s="14" t="s">
         <v>368</v>
       </c>
+      <c r="G209" s="3">
+        <v>1310</v>
+      </c>
+      <c r="H209" s="3">
+        <v>0</v>
+      </c>
+      <c r="I209" s="3">
+        <v>0</v>
+      </c>
+      <c r="J209" s="3">
+        <v>285</v>
+      </c>
+      <c r="K209" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="210" hidden="1" outlineLevel="2">
       <c r="A210" s="16">
@@ -8631,6 +8676,21 @@
       <c r="F210" s="14" t="s">
         <v>369</v>
       </c>
+      <c r="G210" s="3">
+        <v>1355</v>
+      </c>
+      <c r="H210" s="3">
+        <v>0</v>
+      </c>
+      <c r="I210" s="3">
+        <v>0</v>
+      </c>
+      <c r="J210" s="3">
+        <v>405</v>
+      </c>
+      <c r="K210" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="211" hidden="1" outlineLevel="2">
       <c r="A211" s="16">
@@ -8652,16 +8712,16 @@
         <v>372</v>
       </c>
       <c r="G211" s="3">
-        <v>1327</v>
+        <v>1993</v>
       </c>
       <c r="H211" s="3">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="I211" s="3">
         <v>0</v>
       </c>
       <c r="J211" s="3">
-        <v>322</v>
+        <v>501</v>
       </c>
       <c r="K211" s="3">
         <v>0</v>
@@ -8687,16 +8747,16 @@
         <v>374</v>
       </c>
       <c r="G212" s="3">
-        <v>316</v>
+        <v>415</v>
       </c>
       <c r="H212" s="3">
-        <v>20.5</v>
+        <v>10.199999999999989</v>
       </c>
       <c r="I212" s="3">
         <v>0</v>
       </c>
       <c r="J212" s="3">
-        <v>210</v>
+        <v>141</v>
       </c>
       <c r="K212" s="3">
         <v>0</v>
@@ -8722,16 +8782,16 @@
         <v>376</v>
       </c>
       <c r="G213" s="3">
-        <v>287</v>
+        <v>199</v>
       </c>
       <c r="H213" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I213" s="3">
         <v>0</v>
       </c>
       <c r="J213" s="3">
-        <v>121</v>
+        <v>46</v>
       </c>
       <c r="K213" s="3">
         <v>0</v>
@@ -8757,16 +8817,16 @@
         <v>378</v>
       </c>
       <c r="G214" s="3">
-        <v>703</v>
+        <v>333</v>
       </c>
       <c r="H214" s="3">
-        <v>13.5</v>
+        <v>2</v>
       </c>
       <c r="I214" s="3">
         <v>0</v>
       </c>
       <c r="J214" s="3">
-        <v>243</v>
+        <v>81.4</v>
       </c>
       <c r="K214" s="3">
         <v>0</v>
@@ -8792,16 +8852,16 @@
         <v>380</v>
       </c>
       <c r="G215" s="3">
-        <v>140</v>
+        <v>315</v>
       </c>
       <c r="H215" s="3">
-        <v>1</v>
+        <v>3.9500000000000028</v>
       </c>
       <c r="I215" s="3">
         <v>0</v>
       </c>
       <c r="J215" s="3">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="K215" s="3">
         <v>0</v>
@@ -8827,16 +8887,16 @@
         <v>381</v>
       </c>
       <c r="G216" s="3">
-        <v>756</v>
+        <v>716</v>
       </c>
       <c r="H216" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I216" s="3">
         <v>0</v>
       </c>
       <c r="J216" s="3">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="K216" s="3">
         <v>0</v>
@@ -8862,16 +8922,16 @@
         <v>383</v>
       </c>
       <c r="G217" s="3">
-        <v>791</v>
+        <v>1227</v>
       </c>
       <c r="H217" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I217" s="3">
         <v>0</v>
       </c>
       <c r="J217" s="3">
-        <v>237</v>
+        <v>300</v>
       </c>
       <c r="K217" s="3">
         <v>0</v>
@@ -8897,16 +8957,16 @@
         <v>384</v>
       </c>
       <c r="G218" s="3">
-        <v>1152</v>
+        <v>743</v>
       </c>
       <c r="H218" s="3">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I218" s="3">
         <v>0</v>
       </c>
       <c r="J218" s="3">
-        <v>274.45</v>
+        <v>207.35999999999999</v>
       </c>
       <c r="K218" s="3">
         <v>0</v>
@@ -8932,19 +8992,19 @@
         <v>386</v>
       </c>
       <c r="G219" s="3">
-        <v>73</v>
+        <v>632</v>
       </c>
       <c r="H219" s="3">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="I219" s="3">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J219" s="3">
         <v>0</v>
       </c>
       <c r="K219" s="3">
-        <v>62</v>
+        <v>475</v>
       </c>
     </row>
     <row r="220" hidden="1" outlineLevel="2">
@@ -8965,6 +9025,21 @@
       </c>
       <c r="F220" s="14" t="s">
         <v>388</v>
+      </c>
+      <c r="G220" s="3">
+        <v>844</v>
+      </c>
+      <c r="H220" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="I220" s="3">
+        <v>0</v>
+      </c>
+      <c r="J220" s="3">
+        <v>184</v>
+      </c>
+      <c r="K220" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="221" hidden="1" outlineLevel="1" collapsed="1" s="7" customFormat="1">
@@ -8981,19 +9056,19 @@
       <c r="E221" s="8"/>
       <c r="F221" s="8"/>
       <c r="G221" s="7">
-        <v>10043</v>
+        <v>22553</v>
       </c>
       <c r="H221" s="7">
-        <v>314</v>
+        <v>311.65</v>
       </c>
       <c r="I221" s="7">
-        <v>326</v>
+        <v>118</v>
       </c>
       <c r="J221" s="7">
-        <v>5738.45</v>
+        <v>6077.7599999999993</v>
       </c>
       <c r="K221" s="7">
-        <v>487</v>
+        <v>816</v>
       </c>
     </row>
     <row r="222" hidden="1" outlineLevel="2">
@@ -9016,13 +9091,13 @@
         <v>391</v>
       </c>
       <c r="G222" s="3">
-        <v>2060</v>
+        <v>6</v>
       </c>
       <c r="H222" s="3">
         <v>0</v>
       </c>
       <c r="I222" s="3">
-        <v>221</v>
+        <v>1</v>
       </c>
       <c r="J222" s="3">
         <v>0</v>
@@ -9051,13 +9126,13 @@
         <v>392</v>
       </c>
       <c r="G223" s="3">
-        <v>2331</v>
+        <v>473</v>
       </c>
       <c r="H223" s="3">
         <v>0</v>
       </c>
       <c r="I223" s="3">
-        <v>254</v>
+        <v>49</v>
       </c>
       <c r="J223" s="3">
         <v>0</v>
@@ -9085,6 +9160,21 @@
       <c r="F224" s="14" t="s">
         <v>393</v>
       </c>
+      <c r="G224" s="3">
+        <v>12</v>
+      </c>
+      <c r="H224" s="3">
+        <v>0</v>
+      </c>
+      <c r="I224" s="3">
+        <v>2</v>
+      </c>
+      <c r="J224" s="3">
+        <v>0</v>
+      </c>
+      <c r="K224" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="225" hidden="1" outlineLevel="2">
       <c r="A225" s="16">
@@ -9105,21 +9195,6 @@
       <c r="F225" s="14" t="s">
         <v>394</v>
       </c>
-      <c r="G225" s="3">
-        <v>964</v>
-      </c>
-      <c r="H225" s="3">
-        <v>0</v>
-      </c>
-      <c r="I225" s="3">
-        <v>107</v>
-      </c>
-      <c r="J225" s="3">
-        <v>0</v>
-      </c>
-      <c r="K225" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="226" hidden="1" outlineLevel="2">
       <c r="A226" s="16">
@@ -9141,13 +9216,13 @@
         <v>395</v>
       </c>
       <c r="G226" s="3">
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="H226" s="3">
         <v>0</v>
       </c>
       <c r="I226" s="3">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="J226" s="3">
         <v>0</v>
@@ -9176,13 +9251,13 @@
         <v>396</v>
       </c>
       <c r="G227" s="3">
-        <v>3404</v>
+        <v>858</v>
       </c>
       <c r="H227" s="3">
         <v>0</v>
       </c>
       <c r="I227" s="3">
-        <v>368</v>
+        <v>92</v>
       </c>
       <c r="J227" s="3">
         <v>0</v>
@@ -9211,13 +9286,13 @@
         <v>398</v>
       </c>
       <c r="G228" s="3">
-        <v>63</v>
+        <v>419</v>
       </c>
       <c r="H228" s="3">
         <v>0</v>
       </c>
       <c r="I228" s="3">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="J228" s="3">
         <v>0</v>
@@ -9246,13 +9321,13 @@
         <v>399</v>
       </c>
       <c r="G229" s="3">
-        <v>2080</v>
+        <v>439</v>
       </c>
       <c r="H229" s="3">
         <v>0</v>
       </c>
       <c r="I229" s="3">
-        <v>219</v>
+        <v>47</v>
       </c>
       <c r="J229" s="3">
         <v>0</v>
@@ -9280,21 +9355,6 @@
       <c r="F230" s="14" t="s">
         <v>400</v>
       </c>
-      <c r="G230" s="3">
-        <v>733</v>
-      </c>
-      <c r="H230" s="3">
-        <v>0</v>
-      </c>
-      <c r="I230" s="3">
-        <v>0</v>
-      </c>
-      <c r="J230" s="3">
-        <v>65</v>
-      </c>
-      <c r="K230" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="231" hidden="1" outlineLevel="2">
       <c r="A231" s="16">
@@ -9316,19 +9376,19 @@
         <v>402</v>
       </c>
       <c r="G231" s="3">
-        <v>669</v>
+        <v>426</v>
       </c>
       <c r="H231" s="3">
         <v>0</v>
       </c>
       <c r="I231" s="3">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="J231" s="3">
         <v>0</v>
       </c>
       <c r="K231" s="3">
-        <v>117</v>
+        <v>87.47</v>
       </c>
     </row>
     <row r="232" hidden="1" outlineLevel="2">
@@ -9350,6 +9410,21 @@
       <c r="F232" s="14" t="s">
         <v>403</v>
       </c>
+      <c r="G232" s="3">
+        <v>694</v>
+      </c>
+      <c r="H232" s="3">
+        <v>0</v>
+      </c>
+      <c r="I232" s="3">
+        <v>10</v>
+      </c>
+      <c r="J232" s="3">
+        <v>0</v>
+      </c>
+      <c r="K232" s="3">
+        <v>143</v>
+      </c>
     </row>
     <row r="233" hidden="1" outlineLevel="2">
       <c r="A233" s="16">
@@ -9371,13 +9446,13 @@
         <v>407</v>
       </c>
       <c r="G233" s="3">
-        <v>574</v>
+        <v>1095</v>
       </c>
       <c r="H233" s="3">
         <v>0</v>
       </c>
       <c r="I233" s="3">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="J233" s="3">
         <v>0</v>
@@ -9406,19 +9481,19 @@
         <v>408</v>
       </c>
       <c r="G234" s="3">
-        <v>368</v>
+        <v>1136</v>
       </c>
       <c r="H234" s="3">
         <v>0</v>
       </c>
       <c r="I234" s="3">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J234" s="3">
         <v>0</v>
       </c>
       <c r="K234" s="3">
-        <v>86</v>
+        <v>267</v>
       </c>
     </row>
     <row r="235" hidden="1" outlineLevel="2">
@@ -9441,13 +9516,13 @@
         <v>409</v>
       </c>
       <c r="G235" s="3">
-        <v>931</v>
+        <v>938</v>
       </c>
       <c r="H235" s="3">
         <v>0</v>
       </c>
       <c r="I235" s="3">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J235" s="3">
         <v>0</v>
@@ -9476,13 +9551,13 @@
         <v>410</v>
       </c>
       <c r="G236" s="3">
-        <v>331</v>
+        <v>428</v>
       </c>
       <c r="H236" s="3">
         <v>0</v>
       </c>
       <c r="I236" s="3">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="J236" s="3">
         <v>0</v>
@@ -9511,13 +9586,13 @@
         <v>413</v>
       </c>
       <c r="G237" s="3">
-        <v>1459</v>
+        <v>1291</v>
       </c>
       <c r="H237" s="3">
         <v>0</v>
       </c>
       <c r="I237" s="3">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="J237" s="3">
         <v>0</v>
@@ -9546,13 +9621,13 @@
         <v>414</v>
       </c>
       <c r="G238" s="3">
-        <v>1513</v>
+        <v>1340</v>
       </c>
       <c r="H238" s="3">
         <v>0</v>
       </c>
       <c r="I238" s="3">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="J238" s="3">
         <v>0</v>
@@ -9580,21 +9655,6 @@
       <c r="F239" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="G239" s="3">
-        <v>2233</v>
-      </c>
-      <c r="H239" s="3">
-        <v>0</v>
-      </c>
-      <c r="I239" s="3">
-        <v>239</v>
-      </c>
-      <c r="J239" s="3">
-        <v>0</v>
-      </c>
-      <c r="K239" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="240" hidden="1" outlineLevel="2">
       <c r="A240" s="16">
@@ -9615,6 +9675,21 @@
       <c r="F240" s="14" t="s">
         <v>417</v>
       </c>
+      <c r="G240" s="3">
+        <v>27</v>
+      </c>
+      <c r="H240" s="3">
+        <v>0</v>
+      </c>
+      <c r="I240" s="3">
+        <v>1</v>
+      </c>
+      <c r="J240" s="3">
+        <v>0</v>
+      </c>
+      <c r="K240" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="241" hidden="1" outlineLevel="2">
       <c r="A241" s="16">
@@ -9636,19 +9711,19 @@
         <v>419</v>
       </c>
       <c r="G241" s="3">
-        <v>2469</v>
+        <v>2168</v>
       </c>
       <c r="H241" s="3">
         <v>0</v>
       </c>
       <c r="I241" s="3">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="J241" s="3">
         <v>0</v>
       </c>
       <c r="K241" s="3">
-        <v>480</v>
+        <v>392</v>
       </c>
     </row>
     <row r="242" hidden="1" outlineLevel="2">
@@ -9670,21 +9745,6 @@
       <c r="F242" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="G242" s="3">
-        <v>3189</v>
-      </c>
-      <c r="H242" s="3">
-        <v>0</v>
-      </c>
-      <c r="I242" s="3">
-        <v>0</v>
-      </c>
-      <c r="J242" s="3">
-        <v>270</v>
-      </c>
-      <c r="K242" s="3">
-        <v>0</v>
-      </c>
     </row>
     <row r="243" hidden="1" outlineLevel="2">
       <c r="A243" s="16">
@@ -9705,6 +9765,21 @@
       <c r="F243" s="14" t="s">
         <v>421</v>
       </c>
+      <c r="G243" s="3">
+        <v>519</v>
+      </c>
+      <c r="H243" s="3">
+        <v>0</v>
+      </c>
+      <c r="I243" s="3">
+        <v>0</v>
+      </c>
+      <c r="J243" s="3">
+        <v>43</v>
+      </c>
+      <c r="K243" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="244" hidden="1" outlineLevel="2">
       <c r="A244" s="16">
@@ -9725,6 +9800,21 @@
       <c r="F244" s="14" t="s">
         <v>423</v>
       </c>
+      <c r="G244" s="3">
+        <v>316</v>
+      </c>
+      <c r="H244" s="3">
+        <v>0</v>
+      </c>
+      <c r="I244" s="3">
+        <v>0</v>
+      </c>
+      <c r="J244" s="3">
+        <v>33</v>
+      </c>
+      <c r="K244" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="245" hidden="1" outlineLevel="2">
       <c r="A245" s="16">
@@ -9746,13 +9836,13 @@
         <v>425</v>
       </c>
       <c r="G245" s="3">
-        <v>773</v>
+        <v>519</v>
       </c>
       <c r="H245" s="3">
         <v>0</v>
       </c>
       <c r="I245" s="3">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="J245" s="3">
         <v>0</v>
@@ -9780,6 +9870,21 @@
       <c r="F246" s="14" t="s">
         <v>426</v>
       </c>
+      <c r="G246" s="3">
+        <v>558</v>
+      </c>
+      <c r="H246" s="3">
+        <v>0</v>
+      </c>
+      <c r="I246" s="3">
+        <v>59</v>
+      </c>
+      <c r="J246" s="3">
+        <v>0</v>
+      </c>
+      <c r="K246" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="247" hidden="1" outlineLevel="2">
       <c r="A247" s="16">
@@ -9801,13 +9906,13 @@
         <v>427</v>
       </c>
       <c r="G247" s="3">
-        <v>936</v>
+        <v>530</v>
       </c>
       <c r="H247" s="3">
         <v>0</v>
       </c>
       <c r="I247" s="3">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="J247" s="3">
         <v>0</v>
@@ -9830,19 +9935,19 @@
       <c r="E248" s="8"/>
       <c r="F248" s="8"/>
       <c r="G248" s="7">
-        <v>27630</v>
+        <v>14752</v>
       </c>
       <c r="H248" s="7">
         <v>0</v>
       </c>
       <c r="I248" s="7">
-        <v>2329</v>
+        <v>1177</v>
       </c>
       <c r="J248" s="7">
-        <v>335</v>
+        <v>76</v>
       </c>
       <c r="K248" s="7">
-        <v>683</v>
+        <v>895.47</v>
       </c>
     </row>
     <row r="249" hidden="1" outlineLevel="2">
@@ -9865,7 +9970,7 @@
         <v>429</v>
       </c>
       <c r="G249" s="3">
-        <v>3847</v>
+        <v>2822</v>
       </c>
       <c r="H249" s="3">
         <v>0</v>
@@ -9874,7 +9979,7 @@
         <v>0</v>
       </c>
       <c r="J249" s="3">
-        <v>464</v>
+        <v>329</v>
       </c>
       <c r="K249" s="3">
         <v>0</v>
@@ -9900,19 +10005,19 @@
         <v>430</v>
       </c>
       <c r="G250" s="3">
-        <v>639</v>
+        <v>0</v>
       </c>
       <c r="H250" s="3">
         <v>0</v>
       </c>
       <c r="I250" s="3">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="J250" s="3">
         <v>0</v>
       </c>
       <c r="K250" s="3">
-        <v>106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251" hidden="1" outlineLevel="2" s="10" customFormat="1">
@@ -9935,19 +10040,19 @@
         <v>431</v>
       </c>
       <c r="G251" s="10">
-        <v>769</v>
+        <v>1223</v>
       </c>
       <c r="H251" s="10">
         <v>0</v>
       </c>
       <c r="I251" s="10">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J251" s="10">
         <v>0</v>
       </c>
       <c r="K251" s="10">
-        <v>166</v>
+        <v>253</v>
       </c>
     </row>
     <row r="252" hidden="1" outlineLevel="1" collapsed="1" s="7" customFormat="1">
@@ -9964,19 +10069,19 @@
       <c r="E252" s="8"/>
       <c r="F252" s="8"/>
       <c r="G252" s="7">
-        <v>5255</v>
+        <v>4045</v>
       </c>
       <c r="H252" s="7">
         <v>0</v>
       </c>
       <c r="I252" s="7">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="J252" s="7">
-        <v>464</v>
+        <v>329</v>
       </c>
       <c r="K252" s="7">
-        <v>272</v>
+        <v>253</v>
       </c>
     </row>
     <row r="253" ht="21.75" customHeight="1" outlineLevel="1">

</xml_diff>

<commit_message>
Added logs list at footer. Not scrolled
</commit_message>
<xml_diff>
--- a/Console/Main2.xlsx
+++ b/Console/Main2.xlsx
@@ -1846,9 +1846,9 @@
   <dimension ref="A1:F254"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
+      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.3"/>

</xml_diff>